<commit_message>
compared non-normalized and normalized betas (tab "15.14")
</commit_message>
<xml_diff>
--- a/csvs/ruf_betas_042816.xlsx
+++ b/csvs/ruf_betas_042816.xlsx
@@ -9,17 +9,18 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ruf_betas_042816" sheetId="1" r:id="rId1"/>
+    <sheet name="15.14" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="19">
   <si>
     <t>id</t>
   </si>
@@ -71,12 +72,18 @@
   <si>
     <t>se</t>
   </si>
+  <si>
+    <t>non-norm</t>
+  </si>
+  <si>
+    <t>norm</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -207,6 +214,13 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -553,9 +567,17 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -662,7 +684,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EB97B4CA-D825-465A-BCF3-5019827A20AA}" type="CELLRANGE">
+                    <a:fld id="{6CEFD2D9-C714-49E6-9A92-ACCFEAB5095D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -699,7 +721,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1F025509-6126-4E18-8C7C-C75C67CB80C5}" type="CELLRANGE">
+                    <a:fld id="{C34E0D98-04F5-42DC-A670-7E9A74571795}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -736,7 +758,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1DF00F50-3B89-4157-8871-186F1DCCA2A4}" type="CELLRANGE">
+                    <a:fld id="{B3DBD6B6-6D26-441F-958E-61A3DB2D8CDD}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -773,7 +795,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A6FED047-AB30-4938-9F59-6A2C8B39D486}" type="CELLRANGE">
+                    <a:fld id="{6C8A9BA0-DA30-4AC0-B0E8-28928F09460D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -810,7 +832,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E91DC6D0-56BC-4931-A2DA-21A0E4F2C3E8}" type="CELLRANGE">
+                    <a:fld id="{933157C5-050A-4E00-BC54-866C02304F24}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -847,7 +869,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{338EAE69-3623-456A-BD9A-8959E9157466}" type="CELLRANGE">
+                    <a:fld id="{9BB9880E-1CB8-45E6-BE0C-5247B7893483}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -884,7 +906,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{056D4F01-0B72-4EF7-9286-FEFECE31B85D}" type="CELLRANGE">
+                    <a:fld id="{93FDDEBD-F853-4E3A-A523-A9E7C6B30568}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -921,7 +943,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{683DA67F-D787-4350-87E4-5DB73A31C49F}" type="CELLRANGE">
+                    <a:fld id="{EF80DA25-2873-4BD9-9360-6248AF29BB02}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -958,7 +980,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2D2B0801-1F49-4550-BCBB-7A9B5555493F}" type="CELLRANGE">
+                    <a:fld id="{01C89787-E468-4973-8B46-D5B5F7095FF2}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -995,7 +1017,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{97D47347-B015-43E2-AB6D-EF544A8EF67F}" type="CELLRANGE">
+                    <a:fld id="{8E71D56A-C7D2-49CA-BB30-3962B1DCD7A6}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1032,7 +1054,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3EFA9688-6641-4045-8CB9-60376C0EFA62}" type="CELLRANGE">
+                    <a:fld id="{08C86E14-E9C5-4475-A204-C5F35CA17B96}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1092,7 +1114,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showDataLabelsRange val="1"/>
                 <c15:showLeaderLines val="0"/>
               </c:ext>
@@ -1333,11 +1354,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="257255728"/>
-        <c:axId val="257258080"/>
+        <c:axId val="255405056"/>
+        <c:axId val="260578896"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="257255728"/>
+        <c:axId val="255405056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1374,7 +1395,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="257258080"/>
+        <c:crossAx val="260578896"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1382,7 +1403,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="257258080"/>
+        <c:axId val="260578896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1412,7 +1433,7 @@
                     <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                     <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                   </a:rPr>
-                  <a:t>beta coefficient (summer RUF)</a:t>
+                  <a:t>beta coefficient +/- SE (summer RUF)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1481,7 +1502,637 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="257255728"/>
+        <c:crossAx val="255405056"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>normalized UD heights</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'15.14'!$C$1:$M$1</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>intercept</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>beachgrass_dune</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>brackish_marsh</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>coastal_scrub</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>conifer_forest</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>fresh_marsh</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>fruit</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>meadow</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>pasture</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>shrub_swale</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>wooded_swale</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'15.14'!$C$15:$M$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>5.1047600115355599E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.89585272992191E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.25299321073194397</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.2841265562808199E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.0345271371232605E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-2.1867454654730299E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.29305915463189802</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.4702223094826704E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.11629534010793099</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.14426322678995099</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.36428000537855398</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="182"/>
+        <c:axId val="352760096"/>
+        <c:axId val="352762448"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="352760096"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="352762448"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="352762448"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="352760096"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>non-normalized</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> UD heights</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'15.14'!$C$1:$M$1</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>intercept</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>beachgrass_dune</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>brackish_marsh</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>coastal_scrub</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>conifer_forest</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>fresh_marsh</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>fruit</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>meadow</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>pasture</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>shrub_swale</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>wooded_swale</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'15.14'!$C$16:$M$16</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>3.940745E-7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.742962E-7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.0785129999999998E-6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.455394E-7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.5710529999999998E-7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.5049179999999998E-7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.1808029999999998E-6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.3680519999999999E-7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.314087E-7</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.194592E-6</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.5685319999999998E-6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="182"/>
+        <c:axId val="358254208"/>
+        <c:axId val="358245192"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="358254208"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="358245192"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="358245192"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="358254208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1570,7 +2221,1097 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2080,15 +3821,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>295276</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:colOff>228601</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>323850</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>109537</xdr:rowOff>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2102,6 +3843,71 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>147637</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>404812</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>309562</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>90487</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2375,11 +4181,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="12" max="12" width="12.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
@@ -3193,4 +5002,277 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H51" sqref="H51"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="6" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15">
+        <v>5.1047600115355599E-2</v>
+      </c>
+      <c r="D15">
+        <v>1.89585272992191E-2</v>
+      </c>
+      <c r="E15">
+        <v>0.25299321073194397</v>
+      </c>
+      <c r="F15">
+        <v>4.2841265562808199E-2</v>
+      </c>
+      <c r="G15">
+        <v>9.0345271371232605E-2</v>
+      </c>
+      <c r="H15">
+        <v>-2.1867454654730299E-2</v>
+      </c>
+      <c r="I15">
+        <v>0.29305915463189802</v>
+      </c>
+      <c r="J15">
+        <v>9.4702223094826704E-2</v>
+      </c>
+      <c r="K15">
+        <v>0.11629534010793099</v>
+      </c>
+      <c r="L15">
+        <v>0.14426322678995099</v>
+      </c>
+      <c r="M15">
+        <v>0.36428000537855398</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="5">
+        <v>3.940745E-7</v>
+      </c>
+      <c r="D16" s="5">
+        <v>1.742962E-7</v>
+      </c>
+      <c r="E16" s="5">
+        <v>2.0785129999999998E-6</v>
+      </c>
+      <c r="F16" s="5">
+        <v>4.455394E-7</v>
+      </c>
+      <c r="G16" s="5">
+        <v>7.5710529999999998E-7</v>
+      </c>
+      <c r="H16" s="1">
+        <v>2.5049179999999998E-7</v>
+      </c>
+      <c r="I16" s="1">
+        <v>2.1808029999999998E-6</v>
+      </c>
+      <c r="J16" s="1">
+        <v>9.3680519999999999E-7</v>
+      </c>
+      <c r="K16" s="1">
+        <v>9.314087E-7</v>
+      </c>
+      <c r="L16" s="1">
+        <v>1.194592E-6</v>
+      </c>
+      <c r="M16" s="1">
+        <v>3.5685319999999998E-6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="5">
+        <f>C16*100000000</f>
+        <v>39.407449999999997</v>
+      </c>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="2"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="2"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="2"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="2"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="2"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="2"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="2"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="2"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="2"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="2"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="2"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="2"/>
+      <c r="B30" s="4"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="2"/>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>